<commit_message>
Base com as noticias de todos os ativos e código de scrap
</commit_message>
<xml_diff>
--- a/data/BaseRefAtivos.xlsx
+++ b/data/BaseRefAtivos.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuelgandra/Desktop/Projetos /TesteQuant/QuantumSpreadHunters---Quantamental/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F48F3F-CBCC-1B41-B9CC-24EC993F20E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Faça uma lista de TODOS os pote" sheetId="1" r:id="rId4"/>
+    <sheet name="Faça uma lista de TODOS os pote" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="202">
   <si>
     <t>Empresa</t>
   </si>
@@ -491,32 +500,172 @@
   </si>
   <si>
     <t>ABNB</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/microsoft-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/google-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/amazon-com-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/nvidia-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/meta-platforms-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/tesla-motors-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/berkshire-hathaway-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/eli-lilly-and-company-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/visa-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/jp-morgan-chase-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/exxon-mobil-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/johnson-johnson-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/mastercard-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/procter-gamble-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/costco-whsl-corp-new-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/bank-of-america-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/netflix-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/adv-micro-device-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/coca-cola-co-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/pepsico-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/wal-mart-stores-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/mcdonalds-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/disney-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/caterpillar-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/intel-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/cisco-sys-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/oracle-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/salesforce-com-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/adobe-sys-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/nike-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/starbucks-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/boeing-co-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/goldman-sachs-group-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/morgan-stanley-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/ford-motor-co-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/gen-motors-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/pfizer-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/chevron-corp-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/paypal-holdings-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/coinbase-global-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/uber-technologies-inc-news</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/airbnb-inc-news</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -524,42 +673,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -749,20 +904,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -802,7 +962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -818,9 +978,11 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4">
+      <c r="F3" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -836,8 +998,11 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="F4" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -853,8 +1018,11 @@
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="F5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -870,8 +1038,11 @@
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -887,8 +1058,11 @@
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -904,8 +1078,11 @@
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -921,8 +1098,11 @@
       <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -938,8 +1118,11 @@
       <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -955,8 +1138,11 @@
       <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="F11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -972,8 +1158,11 @@
       <c r="E12" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="F12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -989,8 +1178,11 @@
       <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="F13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1006,8 +1198,11 @@
       <c r="E14" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="F14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1023,8 +1218,11 @@
       <c r="E15" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="F15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1040,8 +1238,11 @@
       <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="F16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -1057,8 +1258,11 @@
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="F17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -1074,8 +1278,11 @@
       <c r="E18" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="F18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1091,8 +1298,11 @@
       <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="F19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>75</v>
       </c>
@@ -1108,8 +1318,11 @@
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="F20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -1125,8 +1338,11 @@
       <c r="E21" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="F21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>81</v>
       </c>
@@ -1142,8 +1358,11 @@
       <c r="E22" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="F22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
@@ -1159,8 +1378,11 @@
       <c r="E23" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="F23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
@@ -1176,8 +1398,11 @@
       <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="F24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
@@ -1193,8 +1418,11 @@
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="F25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>95</v>
       </c>
@@ -1210,8 +1438,11 @@
       <c r="E26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="F26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
@@ -1227,8 +1458,11 @@
       <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="F27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>102</v>
       </c>
@@ -1244,8 +1478,11 @@
       <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="F28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>105</v>
       </c>
@@ -1261,8 +1498,11 @@
       <c r="E29" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="F29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>108</v>
       </c>
@@ -1278,8 +1518,11 @@
       <c r="E30" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="F30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
@@ -1295,8 +1538,11 @@
       <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>114</v>
       </c>
@@ -1312,8 +1558,11 @@
       <c r="E32" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33">
+      <c r="F32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>118</v>
       </c>
@@ -1329,8 +1578,11 @@
       <c r="E33" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34">
+      <c r="F33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
@@ -1346,8 +1598,11 @@
       <c r="E34" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35">
+      <c r="F34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>125</v>
       </c>
@@ -1363,8 +1618,11 @@
       <c r="E35" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36">
+      <c r="F35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>128</v>
       </c>
@@ -1380,8 +1638,11 @@
       <c r="E36" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37">
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>131</v>
       </c>
@@ -1397,8 +1658,11 @@
       <c r="E37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38">
+      <c r="F37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>135</v>
       </c>
@@ -1414,8 +1678,11 @@
       <c r="E38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39">
+      <c r="F38" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>138</v>
       </c>
@@ -1431,8 +1698,11 @@
       <c r="E39" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40">
+      <c r="F39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>141</v>
       </c>
@@ -1448,8 +1718,11 @@
       <c r="E40" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41">
+      <c r="F40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>144</v>
       </c>
@@ -1465,8 +1738,11 @@
       <c r="E41" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42">
+      <c r="F41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>148</v>
       </c>
@@ -1482,8 +1758,11 @@
       <c r="E42" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43">
+      <c r="F42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>152</v>
       </c>
@@ -1499,8 +1778,11 @@
       <c r="E43" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44">
+      <c r="F43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>156</v>
       </c>
@@ -1516,11 +1798,17 @@
       <c r="E44" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F44" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{6AE6B1E4-23CA-4049-9392-D60ABCFFFB8F}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{DA28A119-76B1-5F4A-B607-D28F5E1D9028}"/>
+    <hyperlink ref="F44" r:id="rId4" xr:uid="{8006384E-0E24-D543-B381-A82789DA5D58}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>